<commit_message>
Added default codeword sets of Large(200) and Small(80)
</commit_message>
<xml_diff>
--- a/Documentation/Data/200Codewords.xlsx
+++ b/Documentation/Data/200Codewords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531500\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GDP\Project\Documentation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EE6E6931-8853-461E-AF7F-0622E468EDFC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C930C989-2446-4391-B97D-36FFADE5B361}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C44E7D91-EDC8-48E1-9530-79DC7E5796F6}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
   <si>
     <t>Africa</t>
   </si>
@@ -997,7 +997,7 @@
   <dimension ref="A1:B203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1016,7 +1016,9 @@
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">

</xml_diff>